<commit_message>
Added "Sentiment on Performance" analysis
</commit_message>
<xml_diff>
--- a/Sredictio Data Tracking.xlsx
+++ b/Sredictio Data Tracking.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guest1/PycharmProjects/Sredictio-V2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guest1/PycharmProjects/Sredictio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54417C7-8659-2849-84EC-850974AD875E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFC667F-68FF-614E-A67B-018A5B025EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="460" windowWidth="23660" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reward Function VS Net Worth" sheetId="5" r:id="rId1"/>
     <sheet name="Reward Function Analysis" sheetId="7" r:id="rId2"/>
-    <sheet name="Training Data on Performance" sheetId="9" r:id="rId3"/>
+    <sheet name="Sentiment on Performance" sheetId="10" r:id="rId3"/>
+    <sheet name="Training Data on Performance" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Reward Function VS Net Worth'!$A$4:$J$8</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="63">
   <si>
     <t>Training Data</t>
   </si>
@@ -424,6 +425,90 @@
         <rFont val="Helvetica Neue (Body)"/>
       </rPr>
       <t>FOLDER.</t>
+    </r>
+  </si>
+  <si>
+    <t>TRAINING DATA WITH SENTIMENT
+(100K STEPS)</t>
+  </si>
+  <si>
+    <t>TRAINING DATA WITHOUT SENTIMENT
+(100K STEPS)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ALL FILES USED FOR THIS TEST CAN BE FOUND UNDER THE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="American Typewriter"/>
+        <family val="1"/>
+      </rPr>
+      <t>SoP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+FOLDER.</t>
+    </r>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>COMMENTARY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sentiment data does have a positive impact on the performance of the model
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>From the data gathered above, the AVERAGE, MEDIAN and TOTAL were all higher than the non-sentiment data. Granted, the STDEV for the non-sentiment data is lower than that of the sentiment data. However, the low STDEV implies that the possible scores obtained by the non-sentiment data will all be low. Hence, sentiment data is still prefered.</t>
     </r>
   </si>
 </sst>
@@ -566,7 +651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -644,13 +729,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -729,6 +825,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -744,41 +879,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -807,23 +918,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1984,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAECFE35-9265-B04F-8DDD-FAC2A590EDFC}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -1997,52 +2126,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:13" ht="14">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="13" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="12" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -2076,10 +2205,10 @@
         <v>3</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="28"/>
+      <c r="M4" s="41"/>
     </row>
     <row r="5" spans="1:13" ht="14">
       <c r="A5" s="3" t="s">
@@ -2274,32 +2403,32 @@
     </row>
     <row r="12" spans="1:13" ht="13" customHeight="1"/>
     <row r="13" spans="1:13">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:13" ht="13" customHeight="1">
       <c r="A15" s="5" t="s">
@@ -2332,10 +2461,10 @@
       <c r="J15" s="6">
         <v>15.432</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="30"/>
+      <c r="M15" s="43"/>
     </row>
     <row r="16" spans="1:13" ht="14">
       <c r="A16" s="5" t="s">
@@ -2541,52 +2670,52 @@
       <c r="A22" s="15"/>
     </row>
     <row r="24" spans="1:13" ht="24" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" spans="1:13" ht="24" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34" t="s">
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
     </row>
     <row r="27" spans="1:13" ht="14">
       <c r="A27" s="3" t="s">
@@ -2619,10 +2748,10 @@
       <c r="J27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L27" s="29" t="s">
+      <c r="L27" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="30"/>
+      <c r="M27" s="43"/>
     </row>
     <row r="28" spans="1:13" ht="14" customHeight="1">
       <c r="A28" s="3" t="s">
@@ -2815,32 +2944,32 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="40"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="33"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="37"/>
     </row>
     <row r="38" spans="1:13" ht="14">
       <c r="A38" s="5" t="s">
@@ -2873,10 +3002,10 @@
       <c r="J38" s="6">
         <v>16.219000000000001</v>
       </c>
-      <c r="L38" s="29" t="s">
+      <c r="L38" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M38" s="30"/>
+      <c r="M38" s="43"/>
     </row>
     <row r="39" spans="1:13" ht="14">
       <c r="A39" s="5" t="s">
@@ -3076,19 +3205,19 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="13" customHeight="1">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="F47" s="27" t="s">
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="F47" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
     </row>
     <row r="48" spans="1:13" ht="14">
       <c r="A48" s="10"/>
@@ -3101,11 +3230,11 @@
       <c r="D48" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
     </row>
     <row r="49" spans="1:10" ht="14">
       <c r="A49" s="13" t="s">
@@ -3123,11 +3252,11 @@
         <f>SUM(B$9:D$9) + SUM(B$19:D$19) +SUM(B$32:D$32) + SUM(B$42:D$42)</f>
         <v>41</v>
       </c>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
     </row>
     <row r="50" spans="1:10" ht="14">
       <c r="A50" s="13" t="s">
@@ -3145,11 +3274,11 @@
         <f>SUM(E9:G9) + SUM(E19:G19) + SUM(E32:G32) + SUM(E42:G42)</f>
         <v>50</v>
       </c>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
     </row>
     <row r="51" spans="1:10" ht="14">
       <c r="A51" s="13" t="s">
@@ -3167,11 +3296,11 @@
         <f>SUM(H9:J9) + SUM(H19:J19) + SUM(H32:J32) + SUM(H42:J42)</f>
         <v>89</v>
       </c>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
     </row>
     <row r="52" spans="1:10" ht="14">
       <c r="A52" s="13" t="s">
@@ -3189,31 +3318,31 @@
         <f>SUM(B$9:J$9) + SUM(B$19:J$19) +SUM(B$32:J$32) + SUM(B$42:J$42)</f>
         <v>180</v>
       </c>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="40"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
     </row>
     <row r="55" spans="1:10" ht="14">
       <c r="A55" s="10"/>
@@ -3226,11 +3355,11 @@
       <c r="D55" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
     </row>
     <row r="56" spans="1:10" ht="14">
       <c r="A56" s="13" t="s">
@@ -3248,11 +3377,11 @@
         <f>SUM(B21:D21) + SUM(B44:D44)</f>
         <v>5</v>
       </c>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
     </row>
     <row r="57" spans="1:10" ht="14">
       <c r="A57" s="13" t="s">
@@ -3270,11 +3399,11 @@
         <f>SUM(E21:G21) + SUM(E44:G44)</f>
         <v>-10</v>
       </c>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="40"/>
     </row>
     <row r="58" spans="1:10" ht="14">
       <c r="A58" s="13" t="s">
@@ -3292,11 +3421,11 @@
         <f>SUM(H21:J21) + SUM(H44:J44)</f>
         <v>5</v>
       </c>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
     </row>
     <row r="59" spans="1:10" ht="14">
       <c r="A59" s="13" t="s">
@@ -3314,35 +3443,28 @@
         <f>SUM(D56:D58)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="40"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="F60" s="27"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="40"/>
+      <c r="J60" s="40"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="40"/>
+      <c r="J61" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="F47:J61"/>
@@ -3357,6 +3479,13 @@
     <mergeCell ref="A26:J26"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -3370,8 +3499,8 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3381,38 +3510,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="48" customHeight="1">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" ht="12" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
     </row>
     <row r="3" spans="1:11" ht="13" customHeight="1">
       <c r="A3" s="17" t="s">
@@ -3590,19 +3719,19 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
     </row>
     <row r="10" spans="1:11" ht="13" customHeight="1">
       <c r="A10" s="18" t="s">
@@ -3745,23 +3874,23 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52" t="s">
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:11" ht="14">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="47" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -3776,7 +3905,7 @@
       <c r="F16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="47" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="19" t="s">
@@ -3793,7 +3922,7 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" s="52"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="21">
         <f>AVERAGE(B4:F4)</f>
         <v>52.814600000000006</v>
@@ -3810,7 +3939,7 @@
         <f>C17*5</f>
         <v>264.07300000000004</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="21">
         <f>AVERAGE(G4:K4)</f>
         <v>23.332600000000003</v>
@@ -3829,7 +3958,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="14">
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -3844,7 +3973,7 @@
       <c r="F18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="47" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="19" t="s">
@@ -3861,7 +3990,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="B19" s="52"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="21">
         <f>AVERAGE(B10:F10)</f>
         <v>36.681200000000004</v>
@@ -3878,7 +4007,7 @@
         <f>C19*5</f>
         <v>183.40600000000001</v>
       </c>
-      <c r="G19" s="52"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="21">
         <f>AVERAGE(G10:K10)</f>
         <v>19.895800000000001</v>
@@ -3897,19 +4026,19 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
     </row>
     <row r="22" spans="1:11" ht="14">
       <c r="A22" s="25" t="s">
@@ -3983,281 +4112,271 @@
     </row>
     <row r="24" spans="1:11" ht="14" customHeight="1"/>
     <row r="25" spans="1:11">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48" t="s">
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="47"/>
-      <c r="B26" s="49">
+      <c r="A26" s="52"/>
+      <c r="B26" s="54">
         <f>SUM(B22:F23)</f>
         <v>34</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="49">
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="54">
         <f>SUM(G22:K23)</f>
         <v>76</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="51"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="56"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="23"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="44"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="44"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="44"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="44"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="44"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
     <mergeCell ref="A28:K44"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A25:A26"/>
@@ -4265,6 +4384,16 @@
     <mergeCell ref="G25:K25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="G26:K26"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -4275,11 +4404,524 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2A58A4-3406-A44B-A7F6-7945BFECF97B}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="40" customHeight="1">
+      <c r="A1" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="58"/>
+      <c r="L1" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="59"/>
+    </row>
+    <row r="2" spans="1:13" ht="14" customHeight="1">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="62"/>
+      <c r="G2" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+    </row>
+    <row r="3" spans="1:13" ht="14">
+      <c r="A3" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="21">
+        <v>22.024999999999999</v>
+      </c>
+      <c r="C3" s="21">
+        <v>50.421999999999997</v>
+      </c>
+      <c r="D3" s="21">
+        <v>35.448</v>
+      </c>
+      <c r="E3" s="21">
+        <v>26.71</v>
+      </c>
+      <c r="F3" s="62"/>
+      <c r="G3" s="60">
+        <f>STDEV(B3:E3)</f>
+        <v>12.487820823372909</v>
+      </c>
+      <c r="H3" s="66">
+        <f>AVERAGE(B3:E3)</f>
+        <v>33.651250000000005</v>
+      </c>
+      <c r="I3" s="21">
+        <f>MEDIAN(B3:E3)</f>
+        <v>31.079000000000001</v>
+      </c>
+      <c r="J3" s="21">
+        <f>SUM(B3:E3)</f>
+        <v>134.60500000000002</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+    </row>
+    <row r="4" spans="1:13" ht="14">
+      <c r="A4" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="21">
+        <v>21.471</v>
+      </c>
+      <c r="C4" s="21">
+        <v>35.331000000000003</v>
+      </c>
+      <c r="D4" s="21">
+        <v>28.087</v>
+      </c>
+      <c r="E4" s="21">
+        <v>17.619</v>
+      </c>
+      <c r="F4" s="62"/>
+      <c r="G4" s="60">
+        <f>STDEV(B4:E4)</f>
+        <v>7.7807372401334716</v>
+      </c>
+      <c r="H4" s="60">
+        <f>AVERAGE(B4:E4)</f>
+        <v>25.627000000000002</v>
+      </c>
+      <c r="I4" s="21">
+        <f>MEDIAN(B4:E4)</f>
+        <v>24.779</v>
+      </c>
+      <c r="J4" s="21">
+        <f>SUM(B4:E4)</f>
+        <v>102.50800000000001</v>
+      </c>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="62"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+    </row>
+    <row r="6" spans="1:13" ht="40" customHeight="1">
+      <c r="A6" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="61"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+    </row>
+    <row r="7" spans="1:13" ht="14">
+      <c r="A7" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="62"/>
+      <c r="G7" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+    </row>
+    <row r="8" spans="1:13" ht="14">
+      <c r="A8" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="21">
+        <v>21.372</v>
+      </c>
+      <c r="C8" s="21">
+        <v>43.618000000000002</v>
+      </c>
+      <c r="D8" s="21">
+        <v>35.222999999999999</v>
+      </c>
+      <c r="E8" s="21">
+        <v>22.207000000000001</v>
+      </c>
+      <c r="F8" s="62"/>
+      <c r="G8" s="60">
+        <f>STDEV(B8:E8)</f>
+        <v>10.746143277163815</v>
+      </c>
+      <c r="H8" s="60">
+        <f>AVERAGE(B8:E8)</f>
+        <v>30.605000000000004</v>
+      </c>
+      <c r="I8" s="21">
+        <f>MEDIAN(B8:E8)</f>
+        <v>28.715</v>
+      </c>
+      <c r="J8" s="21">
+        <f>SUM(B8:E8)</f>
+        <v>122.42000000000002</v>
+      </c>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+    </row>
+    <row r="9" spans="1:13" ht="14">
+      <c r="A9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="21">
+        <v>26.492999999999999</v>
+      </c>
+      <c r="C9" s="21">
+        <v>28.417000000000002</v>
+      </c>
+      <c r="D9" s="21">
+        <v>16.315000000000001</v>
+      </c>
+      <c r="E9" s="21">
+        <v>21.984000000000002</v>
+      </c>
+      <c r="G9" s="60">
+        <f>STDEV(B9:E9)</f>
+        <v>5.3820999232022153</v>
+      </c>
+      <c r="H9" s="60">
+        <f>AVERAGE(B9:E9)</f>
+        <v>23.302250000000001</v>
+      </c>
+      <c r="I9" s="21">
+        <f>MEDIAN(B9:E9)</f>
+        <v>24.238500000000002</v>
+      </c>
+      <c r="J9" s="21">
+        <f>SUM(B9:E9)</f>
+        <v>93.209000000000003</v>
+      </c>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="K10" s="62"/>
+    </row>
+    <row r="11" spans="1:13" ht="13" customHeight="1">
+      <c r="A11" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="67"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="68"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="67"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="68"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="67"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="67"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="68"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="67"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="67"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A11:J16"/>
+    <mergeCell ref="L1:M9"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0460D6A5-5A34-E54D-8EB7-DEDB2AF9D22A}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4288,20 +4930,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-    </row>
-    <row r="2" spans="1:13" ht="14">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="L1" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="59"/>
+    </row>
+    <row r="2" spans="1:13" ht="14" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -4332,10 +4978,8 @@
       <c r="J2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="57"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" ht="14">
       <c r="A3" s="25" t="s">
@@ -4368,8 +5012,8 @@
       <c r="J3" s="21">
         <v>101.858</v>
       </c>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
     </row>
     <row r="4" spans="1:13" ht="14">
       <c r="A4" s="25" t="s">
@@ -4402,8 +5046,8 @@
       <c r="J4" s="21">
         <v>23.844999999999999</v>
       </c>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
     </row>
     <row r="5" spans="1:13" ht="14">
       <c r="A5" s="25" t="s">
@@ -4436,8 +5080,8 @@
       <c r="J5" s="21">
         <v>77.182000000000002</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
     </row>
     <row r="6" spans="1:13" ht="14">
       <c r="A6" s="25" t="s">
@@ -4470,13 +5114,13 @@
       <c r="J6" s="21">
         <v>25.300999999999998</v>
       </c>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="L2:M6"/>
+    <mergeCell ref="L1:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>